<commit_message>
update the DB content and document
</commit_message>
<xml_diff>
--- a/Wiki Stuff/תכולתDB.xlsx
+++ b/Wiki Stuff/תכולתDB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
   <si>
     <t>קטגוריה ראשית</t>
   </si>
@@ -205,13 +205,76 @@
   </si>
   <si>
     <t>qDMAkvsbu6fHi0OJ44mG</t>
+  </si>
+  <si>
+    <t>חפצים אישיים</t>
+  </si>
+  <si>
+    <t>מפתחות</t>
+  </si>
+  <si>
+    <t>ארנק</t>
+  </si>
+  <si>
+    <t>שעון</t>
+  </si>
+  <si>
+    <t>משקפיים</t>
+  </si>
+  <si>
+    <t>זמנים</t>
+  </si>
+  <si>
+    <t>ימים</t>
+  </si>
+  <si>
+    <t>שבועות</t>
+  </si>
+  <si>
+    <t>חודשים</t>
+  </si>
+  <si>
+    <t>שנים</t>
+  </si>
+  <si>
+    <t>BdRHoAdx5Wmtg8AJXVrT</t>
+  </si>
+  <si>
+    <t>טלפון נייד</t>
+  </si>
+  <si>
+    <t>8DQqjrtGiHKg6z5MTFGN</t>
+  </si>
+  <si>
+    <t>6PE3kLmlR5JzjVit3g5O</t>
+  </si>
+  <si>
+    <t>zMfdLWOdClBUJzQnFCTU</t>
+  </si>
+  <si>
+    <t>vyIBUbPNg7jIfpCdxPGg</t>
+  </si>
+  <si>
+    <t>iqHjGsiXwDBCXFkUc8Xv</t>
+  </si>
+  <si>
+    <t>עמודים מיוחדים</t>
+  </si>
+  <si>
+    <t>מספרים</t>
+  </si>
+  <si>
+    <t>עמודים רגילים</t>
+  </si>
+  <si>
+    <t>סקלת כאב</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,16 +305,60 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -431,51 +538,405 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A2:K67"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -790,559 +1251,1007 @@
     <col min="10" max="10" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1"/>
-    <row r="2" spans="1:10">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="1:10" ht="15" thickBot="1"/>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B3" s="89" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="91"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1">
+      <c r="B4" s="92"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="93"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J5" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1">
-      <c r="B4" s="6" t="s">
+    <row r="6" spans="1:10" ht="15" thickBot="1">
+      <c r="B6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="B7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
-    </row>
-    <row r="5" spans="1:10" ht="15">
-      <c r="B5" s="19"/>
-      <c r="C5" s="6" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" s="16"/>
+      <c r="C8" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="101"/>
+    </row>
+    <row r="9" spans="1:10" ht="15">
+      <c r="B9" s="16"/>
+      <c r="C9" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="4" t="s">
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="60"/>
+      <c r="J9" s="62" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15">
-      <c r="B6" s="19"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+    <row r="10" spans="1:10" ht="15">
+      <c r="B10" s="16"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="4" t="s">
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="55" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15">
-      <c r="B7" s="19"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+    <row r="11" spans="1:10" ht="15">
+      <c r="B11" s="16"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="4" t="s">
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15">
-      <c r="B8" s="19"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
+    <row r="12" spans="1:10" ht="15">
+      <c r="B12" s="16"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="4" t="s">
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="55" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15">
-      <c r="B9" s="19"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
+    <row r="13" spans="1:10" ht="15">
+      <c r="B13" s="16"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="4" t="s">
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="55" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B10" s="19"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="2" t="s">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1">
+      <c r="B14" s="16"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="4" t="s">
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="58" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15">
-      <c r="B11" s="19"/>
-      <c r="C11" s="6" t="s">
+    <row r="15" spans="1:10" ht="15">
+      <c r="B15" s="16"/>
+      <c r="C15" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="4" t="s">
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="28"/>
+      <c r="J15" s="64" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15">
-      <c r="B12" s="19"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15">
-      <c r="B13" s="19"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15">
-      <c r="B14" s="19"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B15" s="19"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15">
       <c r="A16" s="1"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="29"/>
+      <c r="J16" s="56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15">
+      <c r="B17" s="16"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="29"/>
+      <c r="J17" s="56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15">
+      <c r="B18" s="16"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="29"/>
+      <c r="J18" s="56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B19" s="16"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="33"/>
+      <c r="J19" s="66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15">
+      <c r="B20" s="16"/>
+      <c r="C20" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="4" t="s">
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="54" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15">
-      <c r="B17" s="19"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
+    <row r="21" spans="2:10" ht="15">
+      <c r="B21" s="16"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="4" t="s">
+      <c r="G21" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="36"/>
+      <c r="J21" s="55" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15">
-      <c r="B18" s="19"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
+    <row r="22" spans="2:10" ht="15">
+      <c r="B22" s="16"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="4" t="s">
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="55" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15">
-      <c r="B19" s="19"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
+    <row r="23" spans="2:10" ht="15">
+      <c r="B23" s="16"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="4" t="s">
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="55" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B20" s="19"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="2" t="s">
+    <row r="24" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B24" s="16"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="4" t="s">
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="58" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15">
-      <c r="B21" s="8"/>
-      <c r="C21" s="5" t="s">
+    <row r="25" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B25" s="16"/>
+      <c r="C25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="4" t="s">
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="72"/>
+      <c r="J25" s="74" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15">
-      <c r="B22" s="8"/>
-      <c r="C22" s="2" t="s">
+    <row r="26" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B26" s="19"/>
+      <c r="C26" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="4" t="s">
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="68"/>
+      <c r="J26" s="70" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="8"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="8"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="2:10" ht="15" thickBot="1">
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="2:10" ht="15">
-      <c r="B26" s="5" t="s">
+    <row r="27" spans="2:10">
+      <c r="B27" s="19"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="101"/>
+    </row>
+    <row r="28" spans="2:10" ht="15" thickBot="1">
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="102"/>
+      <c r="H28" s="102"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="103"/>
+    </row>
+    <row r="29" spans="2:10" ht="15">
+      <c r="B29" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="4" t="s">
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="75" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="15">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2" t="s">
+    <row r="30" spans="2:10" ht="15">
+      <c r="B30" s="76"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="4" t="s">
+      <c r="G30" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="41"/>
+      <c r="J30" s="77" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="15">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2" t="s">
+    <row r="31" spans="2:10" ht="15">
+      <c r="B31" s="76"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="4" t="s">
+      <c r="G31" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="41"/>
+      <c r="J31" s="77" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="15">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2" t="s">
+    <row r="32" spans="2:10" ht="15">
+      <c r="B32" s="76"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" s="2"/>
-      <c r="J29" s="4" t="s">
+      <c r="G32" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" s="41"/>
+      <c r="J32" s="77" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="15">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2" t="s">
+    <row r="33" spans="2:11" ht="15">
+      <c r="B33" s="76"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="4" t="s">
+      <c r="G33" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="41"/>
+      <c r="J33" s="77" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="15">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2" t="s">
+    <row r="34" spans="2:11" ht="15">
+      <c r="B34" s="76"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I31" s="2"/>
-      <c r="J31" s="4" t="s">
+      <c r="G34" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="41"/>
+      <c r="J34" s="77" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="15">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2" t="s">
+    <row r="35" spans="2:11" ht="15">
+      <c r="B35" s="76"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32" s="2"/>
-      <c r="J32" s="4" t="s">
+      <c r="G35" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="41"/>
+      <c r="J35" s="77" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="15">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2" t="s">
+    <row r="36" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B36" s="78"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="79"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I33" s="2"/>
-      <c r="J33" s="4" t="s">
+      <c r="G36" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="79"/>
+      <c r="J36" s="81" t="s">
         <v>58</v>
       </c>
     </row>
+    <row r="37" spans="2:11" ht="15">
+      <c r="B37" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="84" t="s">
+        <v>73</v>
+      </c>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="2:11" ht="15">
+      <c r="B38" s="47"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="G38" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="48"/>
+      <c r="J38" s="85" t="s">
+        <v>75</v>
+      </c>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="2:11" ht="15">
+      <c r="B39" s="47"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="48"/>
+      <c r="J39" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="2:11" ht="15">
+      <c r="B40" s="47"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="48"/>
+      <c r="J40" s="85" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="15">
+      <c r="B41" s="47"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="48"/>
+      <c r="J41" s="85" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B42" s="50"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="G42" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" s="51"/>
+      <c r="J42" s="86" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="2:11">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="2:10" ht="15">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="2:10" ht="15">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="2"/>
+    </row>
+    <row r="56" spans="2:10" ht="15">
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="2:10" ht="15" thickBot="1"/>
+    <row r="58" spans="2:10">
+      <c r="B58" s="89" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" s="90"/>
+      <c r="D58" s="90"/>
+      <c r="E58" s="90"/>
+      <c r="F58" s="90"/>
+      <c r="G58" s="90"/>
+      <c r="H58" s="90"/>
+      <c r="I58" s="90"/>
+      <c r="J58" s="91"/>
+    </row>
+    <row r="59" spans="2:10" ht="15" thickBot="1">
+      <c r="B59" s="92"/>
+      <c r="C59" s="88"/>
+      <c r="D59" s="88"/>
+      <c r="E59" s="88"/>
+      <c r="F59" s="88"/>
+      <c r="G59" s="88"/>
+      <c r="H59" s="88"/>
+      <c r="I59" s="88"/>
+      <c r="J59" s="93"/>
+    </row>
+    <row r="60" spans="2:10">
+      <c r="B60" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" ht="15" thickBot="1">
+      <c r="B61" s="6"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="12"/>
+    </row>
+    <row r="62" spans="2:10" ht="15">
+      <c r="B62" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="H62" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="I62" s="23"/>
+      <c r="J62" s="87"/>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="B63" s="26"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G63" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H63" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I63" s="24"/>
+      <c r="J63" s="83"/>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="B64" s="26"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G64" s="24"/>
+      <c r="H64" s="24"/>
+      <c r="I64" s="24"/>
+      <c r="J64" s="83"/>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" s="26"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G65" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I65" s="24"/>
+      <c r="J65" s="83"/>
+    </row>
+    <row r="66" spans="2:10" ht="15" thickBot="1">
+      <c r="B66" s="94"/>
+      <c r="C66" s="95"/>
+      <c r="D66" s="95"/>
+      <c r="E66" s="95"/>
+      <c r="F66" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="G66" s="95"/>
+      <c r="H66" s="95"/>
+      <c r="I66" s="95"/>
+      <c r="J66" s="96"/>
+    </row>
+    <row r="67" spans="2:10" ht="15" thickBot="1">
+      <c r="B67" s="97" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="98"/>
+      <c r="D67" s="98"/>
+      <c r="E67" s="98"/>
+      <c r="F67" s="98"/>
+      <c r="G67" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="H67" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="I67" s="98"/>
+      <c r="J67" s="100"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
+  <mergeCells count="20">
+    <mergeCell ref="B58:J59"/>
+    <mergeCell ref="B3:J4"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="H60:H61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
adding the hirarchy for sub categories.
</commit_message>
<xml_diff>
--- a/Wiki Stuff/תכולתDB.xlsx
+++ b/Wiki Stuff/תכולתDB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="93">
   <si>
     <t>קטגוריה ראשית</t>
   </si>
@@ -268,6 +268,33 @@
   </si>
   <si>
     <t>סקלת כאב</t>
+  </si>
+  <si>
+    <t>1htM218ibmtwusrEVM7O</t>
+  </si>
+  <si>
+    <t>imageURL</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>parentCategoryID</t>
+  </si>
+  <si>
+    <t>categoryID</t>
+  </si>
+  <si>
+    <t>voiceURL</t>
+  </si>
+  <si>
+    <t>שדות קטגוריה בDB:</t>
+  </si>
+  <si>
+    <t>שדות ביטוי בDB:</t>
   </si>
 </sst>
 </file>
@@ -358,7 +385,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -764,11 +791,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -800,7 +866,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -937,6 +1002,62 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1231,10 +1352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:K67"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1243,7 +1364,7 @@
     <col min="2" max="2" width="24.125" customWidth="1"/>
     <col min="3" max="3" width="13.375" customWidth="1"/>
     <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="17.25" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="8.375" customWidth="1"/>
     <col min="8" max="8" width="6.75" customWidth="1"/>
@@ -1251,756 +1372,748 @@
     <col min="10" max="10" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15" thickBot="1"/>
+    <row r="1" spans="1:10" ht="15" thickBot="1"/>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+      <c r="C2" s="118"/>
+      <c r="E2" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="124" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B3" s="89" t="s">
+      <c r="C3" s="118"/>
+      <c r="E3" s="119" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="122" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="C4" s="118"/>
+      <c r="E4" s="119" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="122" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="C5" s="118"/>
+      <c r="E5" s="119" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="122" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1">
+      <c r="E6" s="120" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="123" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1"/>
+    <row r="8" spans="1:10">
+      <c r="B8" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1">
-      <c r="B4" s="92"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="93"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="B5" s="5" t="s">
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="105"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1">
+      <c r="B9" s="106"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="107"/>
+      <c r="J9" s="108"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C10" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D10" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E10" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F10" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G10" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H10" s="109" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I10" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J10" s="111" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1">
-      <c r="B6" s="6"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="13" t="s">
+    <row r="11" spans="1:10" ht="15" thickBot="1">
+      <c r="B11" s="114"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="112"/>
+    </row>
+    <row r="12" spans="1:10" ht="15">
+      <c r="B12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="117" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="15"/>
+      <c r="C13" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="101"/>
-    </row>
-    <row r="9" spans="1:10" ht="15">
-      <c r="B9" s="16"/>
-      <c r="C9" s="59" t="s">
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="100"/>
+    </row>
+    <row r="14" spans="1:10" ht="15">
+      <c r="B14" s="15"/>
+      <c r="C14" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="60"/>
-      <c r="J9" s="62" t="s">
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="59"/>
+      <c r="J14" s="61" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15">
-      <c r="B10" s="16"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36" t="s">
+    <row r="15" spans="1:10" ht="15">
+      <c r="B15" s="15"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="55" t="s">
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="54" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15">
-      <c r="B11" s="16"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="55" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15">
-      <c r="B12" s="16"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="55" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15">
-      <c r="B13" s="16"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="55" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B14" s="16"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="58" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15">
-      <c r="B15" s="16"/>
-      <c r="C15" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="28"/>
-      <c r="J15" s="64" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15">
       <c r="A16" s="1"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15">
+      <c r="B17" s="15"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15">
+      <c r="B18" s="15"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B19" s="15"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15">
+      <c r="B20" s="15"/>
+      <c r="C20" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="27"/>
+      <c r="J20" s="63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15">
+      <c r="B21" s="15"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="56" t="s">
+      <c r="G21" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="28"/>
+      <c r="J21" s="55" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15">
-      <c r="B17" s="16"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29" t="s">
+    <row r="22" spans="2:10" ht="15">
+      <c r="B22" s="15"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="29"/>
-      <c r="J17" s="56" t="s">
+      <c r="G22" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="28"/>
+      <c r="J22" s="55" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15">
-      <c r="B18" s="16"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29" t="s">
+    <row r="23" spans="2:10" ht="15">
+      <c r="B23" s="15"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="29"/>
-      <c r="J18" s="56" t="s">
+      <c r="G23" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="28"/>
+      <c r="J23" s="55" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B19" s="16"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33" t="s">
+    <row r="24" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B24" s="15"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="33"/>
-      <c r="J19" s="66" t="s">
+      <c r="G24" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="32"/>
+      <c r="J24" s="65" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="15">
-      <c r="B20" s="16"/>
-      <c r="C20" s="34" t="s">
+    <row r="25" spans="2:10" ht="15">
+      <c r="B25" s="15"/>
+      <c r="C25" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="54" t="s">
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15">
-      <c r="B21" s="16"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36" t="s">
+    <row r="26" spans="2:10" ht="15">
+      <c r="B26" s="15"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="55" t="s">
+      <c r="G26" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="35"/>
+      <c r="J26" s="54" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15">
-      <c r="B22" s="16"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36" t="s">
+    <row r="27" spans="2:10" ht="15">
+      <c r="B27" s="15"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="55" t="s">
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15">
-      <c r="B23" s="16"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36" t="s">
+    <row r="28" spans="2:10" ht="15">
+      <c r="B28" s="15"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="55" t="s">
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="54" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B24" s="16"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40" t="s">
+    <row r="29" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B29" s="15"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="58" t="s">
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="57" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B25" s="16"/>
-      <c r="C25" s="71" t="s">
+    <row r="30" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B30" s="15"/>
+      <c r="C30" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="72"/>
-      <c r="J25" s="74" t="s">
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="71"/>
+      <c r="J30" s="73" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B26" s="19"/>
-      <c r="C26" s="67" t="s">
+    <row r="31" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B31" s="18"/>
+      <c r="C31" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="I26" s="68"/>
-      <c r="J26" s="70" t="s">
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="67"/>
+      <c r="J31" s="69" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
-      <c r="B27" s="19"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="101"/>
-    </row>
-    <row r="28" spans="2:10" ht="15" thickBot="1">
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="102"/>
-      <c r="H28" s="102"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="103"/>
-    </row>
-    <row r="29" spans="2:10" ht="15">
-      <c r="B29" s="43" t="s">
+    <row r="32" spans="2:10">
+      <c r="B32" s="18"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="100"/>
+    </row>
+    <row r="33" spans="2:11" ht="15" thickBot="1">
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="101"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="102"/>
+    </row>
+    <row r="34" spans="2:11" ht="15">
+      <c r="B34" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="75" t="s">
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="74" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="15">
-      <c r="B30" s="76"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41" t="s">
+    <row r="35" spans="2:11" ht="15">
+      <c r="B35" s="75"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="G30" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="I30" s="41"/>
-      <c r="J30" s="77" t="s">
+      <c r="G35" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="40"/>
+      <c r="J35" s="76" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="15">
-      <c r="B31" s="76"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41" t="s">
+    <row r="36" spans="2:11" ht="15">
+      <c r="B36" s="75"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="I31" s="41"/>
-      <c r="J31" s="77" t="s">
+      <c r="G36" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="40"/>
+      <c r="J36" s="76" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="15">
-      <c r="B32" s="76"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41" t="s">
+    <row r="37" spans="2:11" ht="15">
+      <c r="B37" s="75"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G32" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32" s="41"/>
-      <c r="J32" s="77" t="s">
+      <c r="G37" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="40"/>
+      <c r="J37" s="76" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="2:11" ht="15">
-      <c r="B33" s="76"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41" t="s">
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="2:11" ht="15">
+      <c r="B38" s="75"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G33" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="I33" s="41"/>
-      <c r="J33" s="77" t="s">
+      <c r="G38" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="40"/>
+      <c r="J38" s="76" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="34" spans="2:11" ht="15">
-      <c r="B34" s="76"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41" t="s">
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="2:11" ht="15">
+      <c r="B39" s="75"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="G34" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="H34" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="I34" s="41"/>
-      <c r="J34" s="77" t="s">
+      <c r="G39" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="40"/>
+      <c r="J39" s="76" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="2:11" ht="15">
-      <c r="B35" s="76"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41" t="s">
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="2:11" ht="15">
+      <c r="B40" s="75"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="G35" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="H35" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="I35" s="41"/>
-      <c r="J35" s="77" t="s">
+      <c r="G40" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="40"/>
+      <c r="J40" s="76" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B36" s="78"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="79"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79" t="s">
+    <row r="41" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B41" s="77"/>
+      <c r="C41" s="78"/>
+      <c r="D41" s="78"/>
+      <c r="E41" s="78"/>
+      <c r="F41" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="G36" s="80" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36" s="80" t="s">
-        <v>9</v>
-      </c>
-      <c r="I36" s="79"/>
-      <c r="J36" s="81" t="s">
+      <c r="G41" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="78"/>
+      <c r="J41" s="80" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="15">
-      <c r="B37" s="45" t="s">
+    <row r="42" spans="2:11" ht="15">
+      <c r="B42" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="84" t="s">
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="83" t="s">
         <v>73</v>
       </c>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="2:11" ht="15">
-      <c r="B38" s="47"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48" t="s">
+    </row>
+    <row r="43" spans="2:11" ht="15">
+      <c r="B43" s="46"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="G38" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="I38" s="48"/>
-      <c r="J38" s="85" t="s">
+      <c r="G43" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="47"/>
+      <c r="J43" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="K38" s="1"/>
-    </row>
-    <row r="39" spans="2:11" ht="15">
-      <c r="B39" s="47"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48" t="s">
+    </row>
+    <row r="44" spans="2:11" ht="15">
+      <c r="B44" s="46"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G39" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="85" t="s">
+      <c r="G44" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" s="47"/>
+      <c r="J44" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="K39" s="1"/>
-    </row>
-    <row r="40" spans="2:11" ht="15">
-      <c r="B40" s="47"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48" t="s">
+    </row>
+    <row r="45" spans="2:11" ht="15">
+      <c r="B45" s="46"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="G40" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="H40" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="I40" s="48"/>
-      <c r="J40" s="85" t="s">
+      <c r="G45" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" s="47"/>
+      <c r="J45" s="84" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="15">
-      <c r="B41" s="47"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48" t="s">
+    <row r="46" spans="2:11" ht="15">
+      <c r="B46" s="46"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="G41" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="H41" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="I41" s="48"/>
-      <c r="J41" s="85" t="s">
+      <c r="G46" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="I46" s="47"/>
+      <c r="J46" s="84" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B42" s="50"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51" t="s">
+    <row r="47" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B47" s="49"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="G42" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="H42" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="I42" s="51"/>
-      <c r="J42" s="86" t="s">
+      <c r="G47" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" s="50"/>
+      <c r="J47" s="85" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="2:11">
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-    </row>
-    <row r="44" spans="2:11">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="2:11">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="2:11">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="2:11">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-    </row>
     <row r="48" spans="2:11">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
     </row>
     <row r="49" spans="2:10">
       <c r="B49" s="2"/>
@@ -2035,11 +2148,11 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="2:10" ht="15">
+    <row r="52" spans="2:10">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="3"/>
+      <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -2057,201 +2170,247 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="2:10" ht="15">
+    <row r="54" spans="2:10">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="3"/>
+      <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
-      <c r="I54" s="3"/>
+      <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="56" spans="2:10" ht="15">
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="2:10" ht="15" thickBot="1"/>
-    <row r="58" spans="2:10">
-      <c r="B58" s="89" t="s">
+    <row r="55" spans="2:10">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+    </row>
+    <row r="57" spans="2:10" ht="15">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" spans="2:10" ht="14.25" customHeight="1">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="2:10" ht="15" customHeight="1">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" spans="2:10" ht="14.25" customHeight="1"/>
+    <row r="61" spans="2:10" ht="15" customHeight="1">
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="2:10" ht="15" thickBot="1"/>
+    <row r="63" spans="2:10" ht="26.25">
+      <c r="B63" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="90"/>
-      <c r="D58" s="90"/>
-      <c r="E58" s="90"/>
-      <c r="F58" s="90"/>
-      <c r="G58" s="90"/>
-      <c r="H58" s="90"/>
-      <c r="I58" s="90"/>
-      <c r="J58" s="91"/>
-    </row>
-    <row r="59" spans="2:10" ht="15" thickBot="1">
-      <c r="B59" s="92"/>
-      <c r="C59" s="88"/>
-      <c r="D59" s="88"/>
-      <c r="E59" s="88"/>
-      <c r="F59" s="88"/>
-      <c r="G59" s="88"/>
-      <c r="H59" s="88"/>
-      <c r="I59" s="88"/>
-      <c r="J59" s="93"/>
-    </row>
-    <row r="60" spans="2:10">
-      <c r="B60" s="5" t="s">
+      <c r="C63" s="89"/>
+      <c r="D63" s="89"/>
+      <c r="E63" s="89"/>
+      <c r="F63" s="89"/>
+      <c r="G63" s="89"/>
+      <c r="H63" s="89"/>
+      <c r="I63" s="89"/>
+      <c r="J63" s="90"/>
+    </row>
+    <row r="64" spans="2:10" ht="27" thickBot="1">
+      <c r="B64" s="91"/>
+      <c r="C64" s="87"/>
+      <c r="D64" s="87"/>
+      <c r="E64" s="87"/>
+      <c r="F64" s="87"/>
+      <c r="G64" s="87"/>
+      <c r="H64" s="87"/>
+      <c r="I64" s="87"/>
+      <c r="J64" s="92"/>
+    </row>
+    <row r="65" spans="2:10" ht="47.25">
+      <c r="B65" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C65" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D65" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E65" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F60" s="7" t="s">
+      <c r="F65" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="9" t="s">
+      <c r="G65" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H60" s="9" t="s">
+      <c r="H65" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I60" s="9" t="s">
+      <c r="I65" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J60" s="11" t="s">
+      <c r="J65" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="2:10" ht="15" thickBot="1">
-      <c r="B61" s="6"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="12"/>
-    </row>
-    <row r="62" spans="2:10" ht="15">
-      <c r="B62" s="22" t="s">
+    <row r="66" spans="2:10" ht="16.5" thickBot="1">
+      <c r="B66" s="6"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="12"/>
+    </row>
+    <row r="67" spans="2:10" ht="15">
+      <c r="B67" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="H62" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="I62" s="23"/>
-      <c r="J62" s="87"/>
-    </row>
-    <row r="63" spans="2:10">
-      <c r="B63" s="26"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24" t="s">
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="H67" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="I67" s="22"/>
+      <c r="J67" s="86"/>
+    </row>
+    <row r="68" spans="2:10">
+      <c r="B68" s="25"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="G63" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H63" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I63" s="24"/>
-      <c r="J63" s="83"/>
-    </row>
-    <row r="64" spans="2:10">
-      <c r="B64" s="26"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24" t="s">
+      <c r="G68" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H68" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I68" s="23"/>
+      <c r="J68" s="82"/>
+    </row>
+    <row r="69" spans="2:10">
+      <c r="B69" s="25"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="G64" s="24"/>
-      <c r="H64" s="24"/>
-      <c r="I64" s="24"/>
-      <c r="J64" s="83"/>
-    </row>
-    <row r="65" spans="2:10">
-      <c r="B65" s="26"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24" t="s">
+      <c r="G69" s="23"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
+      <c r="J69" s="82"/>
+    </row>
+    <row r="70" spans="2:10">
+      <c r="B70" s="25"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G65" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H65" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I65" s="24"/>
-      <c r="J65" s="83"/>
-    </row>
-    <row r="66" spans="2:10" ht="15" thickBot="1">
-      <c r="B66" s="94"/>
-      <c r="C66" s="95"/>
-      <c r="D66" s="95"/>
-      <c r="E66" s="95"/>
-      <c r="F66" s="95" t="s">
+      <c r="G70" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H70" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I70" s="23"/>
+      <c r="J70" s="82"/>
+    </row>
+    <row r="71" spans="2:10" ht="15" thickBot="1">
+      <c r="B71" s="93"/>
+      <c r="C71" s="94"/>
+      <c r="D71" s="94"/>
+      <c r="E71" s="94"/>
+      <c r="F71" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="G66" s="95"/>
-      <c r="H66" s="95"/>
-      <c r="I66" s="95"/>
-      <c r="J66" s="96"/>
-    </row>
-    <row r="67" spans="2:10" ht="15" thickBot="1">
-      <c r="B67" s="97" t="s">
+      <c r="G71" s="94"/>
+      <c r="H71" s="94"/>
+      <c r="I71" s="94"/>
+      <c r="J71" s="95"/>
+    </row>
+    <row r="72" spans="2:10" ht="15" thickBot="1">
+      <c r="B72" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="C67" s="98"/>
-      <c r="D67" s="98"/>
-      <c r="E67" s="98"/>
-      <c r="F67" s="98"/>
-      <c r="G67" s="99" t="s">
-        <v>9</v>
-      </c>
-      <c r="H67" s="99" t="s">
-        <v>9</v>
-      </c>
-      <c r="I67" s="98"/>
-      <c r="J67" s="100"/>
+      <c r="C72" s="97"/>
+      <c r="D72" s="97"/>
+      <c r="E72" s="97"/>
+      <c r="F72" s="97"/>
+      <c r="G72" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="H72" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="I72" s="97"/>
+      <c r="J72" s="99"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B58:J59"/>
-    <mergeCell ref="B3:J4"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="H60:H61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
+  <mergeCells count="10">
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:J9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>